<commit_message>
Map now responsive, functional.
-- Fixed database coordinates (longitudes were positive instead of negative, causing parking lot markers to be placed in western China instead of Lexington)

-- Map now displays blue markers representing available parking lots based on parking form data.

-- Parking lot markers contain clickable labels containing the name of the lot and exact coordinates

-- Implemented function that finds the parking lot that is of shortest distance to the user's location and draws a path between the two markers
</commit_message>
<xml_diff>
--- a/app/data/UK_Parking_Coords.xlsx
+++ b/app/data/UK_Parking_Coords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12703\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klingendoich/UK Courses/#FA24/cs498/498-Project/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ACB3B9C-7EEA-4BF9-975C-1547CE4BF0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126FB50C-1825-5B49-9C36-EE6B69FAE6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{44407656-1C7A-8D4D-AE85-25244241003C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{44407656-1C7A-8D4D-AE85-25244241003C}"/>
   </bookViews>
   <sheets>
     <sheet name="Type" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -489,6 +489,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -530,6 +536,7 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
@@ -871,12 +878,12 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.09765625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -892,7 +899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -900,7 +907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="142.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -908,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -916,7 +923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -924,7 +931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -932,7 +939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -940,7 +947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -948,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -956,7 +963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -964,7 +971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -972,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -980,7 +987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -988,7 +995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -996,7 +1003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1004,7 +1011,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1012,7 +1019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1020,7 +1027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1028,7 +1035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1036,7 +1043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1044,7 +1051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1052,7 +1059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1060,7 +1067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1068,7 +1075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1076,7 +1083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1092,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1100,7 +1107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1108,7 +1115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1116,7 +1123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1124,7 +1131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1132,7 +1139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1140,7 +1147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1148,7 +1155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1156,7 +1163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1164,32 +1171,32 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1204,57 +1211,57 @@
       <selection pane="topRight" activeCell="AL39" sqref="AL39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="5.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="26.5" style="3" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.8984375" style="3" customWidth="1"/>
+    <col min="34" max="34" width="12.83203125" style="3" customWidth="1"/>
     <col min="35" max="37" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="17.5" style="3" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
@@ -1415,7 +1422,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1743,7 +1750,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1907,7 +1914,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2071,7 +2078,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -2235,7 +2242,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -2399,7 +2406,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2563,7 +2570,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2727,7 +2734,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -2891,7 +2898,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -3055,7 +3062,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -3219,7 +3226,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -3383,7 +3390,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -3547,7 +3554,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -3711,7 +3718,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -3875,7 +3882,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -4039,7 +4046,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -4203,7 +4210,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -4367,7 +4374,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -4531,7 +4538,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -4695,7 +4702,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -4859,7 +4866,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -5023,7 +5030,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -5187,7 +5194,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>122</v>
       </c>
@@ -5351,7 +5358,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -5515,7 +5522,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -5679,7 +5686,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -5843,7 +5850,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -6007,7 +6014,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -6171,7 +6178,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -6335,7 +6342,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -6499,7 +6506,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>130</v>
       </c>
@@ -6663,7 +6670,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -6827,7 +6834,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -6991,7 +6998,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -7155,7 +7162,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -7319,7 +7326,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>134</v>
       </c>
@@ -7497,54 +7504,54 @@
       <selection pane="topRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="5.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="4.09765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6.5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="26.5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="26" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.09765625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="17.5" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="14" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>41</v>
       </c>
@@ -7705,7 +7712,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7869,7 +7876,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -8033,7 +8040,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -8197,7 +8204,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -8361,7 +8368,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -8525,7 +8532,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -8689,7 +8696,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -8853,7 +8860,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -9017,7 +9024,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -9181,7 +9188,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -9345,7 +9352,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -9509,7 +9516,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -9673,7 +9680,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -9837,7 +9844,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -10001,7 +10008,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -10165,7 +10172,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -10329,7 +10336,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -10493,7 +10500,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -10657,7 +10664,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -10821,7 +10828,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -10985,7 +10992,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -11149,7 +11156,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -11313,7 +11320,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -11477,7 +11484,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>122</v>
       </c>
@@ -11641,7 +11648,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -11805,7 +11812,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -11969,7 +11976,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -12133,7 +12140,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -12297,7 +12304,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -12461,7 +12468,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -12625,7 +12632,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -12789,7 +12796,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>130</v>
       </c>
@@ -12953,7 +12960,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -13117,7 +13124,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -13281,7 +13288,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -13445,7 +13452,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -13609,7 +13616,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>136</v>
       </c>
@@ -13782,16 +13789,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE90556-68AC-6A42-A95E-5A6F62ADC572}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>137</v>
       </c>
@@ -13799,7 +13806,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
@@ -13807,9 +13814,9 @@
         <v>38.033940000000001</v>
       </c>
       <c r="C2">
-        <v>84.503950000000003</v>
-      </c>
-      <c r="D2" s="6"/>
+        <v>-84.503950000000003</v>
+      </c>
+      <c r="D2" s="8"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -13860,7 +13867,7 @@
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
@@ -13868,10 +13875,11 @@
         <v>38.033749999999998</v>
       </c>
       <c r="C3">
-        <v>84.507390000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.507390000000001</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
@@ -13879,10 +13887,11 @@
         <v>38.042290000000001</v>
       </c>
       <c r="C4">
-        <v>84.501639999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.501639999999995</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
@@ -13890,10 +13899,11 @@
         <v>38.0274</v>
       </c>
       <c r="C5">
-        <v>84.501350000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.501350000000002</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>45</v>
       </c>
@@ -13901,10 +13911,11 @@
         <v>38.03152</v>
       </c>
       <c r="C6">
-        <v>84.510109999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.510109999999997</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -13912,10 +13923,11 @@
         <v>38.039029999999997</v>
       </c>
       <c r="C7">
-        <v>84.505070000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.505070000000003</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>47</v>
       </c>
@@ -13923,10 +13935,11 @@
         <v>38.039250000000003</v>
       </c>
       <c r="C8">
-        <v>84.499420000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.499420000000001</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
@@ -13934,10 +13947,11 @@
         <v>38.029670000000003</v>
       </c>
       <c r="C9">
-        <v>84.505470000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.505470000000003</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
@@ -13945,10 +13959,11 @@
         <v>38.034799999999997</v>
       </c>
       <c r="C10">
-        <v>84.510469999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.510469999999998</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
@@ -13956,10 +13971,11 @@
         <v>38.037640000000003</v>
       </c>
       <c r="C11">
-        <v>84.507769999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.507769999999994</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
@@ -13967,10 +13983,11 @@
         <v>38.017130000000002</v>
       </c>
       <c r="C12">
-        <v>84.508229999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.508229999999998</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
@@ -13978,10 +13995,11 @@
         <v>38.021000000000001</v>
       </c>
       <c r="C13">
-        <v>84.501620000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.501620000000003</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>53</v>
       </c>
@@ -13989,10 +14007,11 @@
         <v>38.02084</v>
       </c>
       <c r="C14">
-        <v>84.502859999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.502859999999998</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -14000,10 +14019,11 @@
         <v>38.01979</v>
       </c>
       <c r="C15">
-        <v>84.502629999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
+        <v>-84.502629999999996</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>55</v>
       </c>
@@ -14011,10 +14031,11 @@
         <v>38.027366000000001</v>
       </c>
       <c r="C16">
-        <v>84.506247999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.506247999999999</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
@@ -14022,10 +14043,11 @@
         <v>38.033586999999997</v>
       </c>
       <c r="C17">
-        <v>84.503843000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.503843000000003</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>57</v>
       </c>
@@ -14033,10 +14055,11 @@
         <v>38.040770999999999</v>
       </c>
       <c r="C18">
-        <v>84.505187000000006</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.505187000000006</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>58</v>
       </c>
@@ -14044,10 +14067,11 @@
         <v>38.034567000000003</v>
       </c>
       <c r="C19">
-        <v>84.511989</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.511989</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>59</v>
       </c>
@@ -14055,10 +14079,11 @@
         <v>38.040120000000002</v>
       </c>
       <c r="C20">
-        <v>84.508309999999994</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.508309999999994</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>60</v>
       </c>
@@ -14066,10 +14091,11 @@
         <v>38.039990000000003</v>
       </c>
       <c r="C21" s="7">
-        <v>84.499290000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.499290000000002</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>61</v>
       </c>
@@ -14077,10 +14103,11 @@
         <v>38.027439999999999</v>
       </c>
       <c r="C22">
-        <v>38.027439999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-38.027439999999999</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>62</v>
       </c>
@@ -14088,10 +14115,11 @@
         <v>38.03152</v>
       </c>
       <c r="C23">
-        <v>84.498310000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.498310000000004</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>63</v>
       </c>
@@ -14099,10 +14127,11 @@
         <v>38.025069999999999</v>
       </c>
       <c r="C24">
-        <v>84.505430000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.505430000000004</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>64</v>
       </c>
@@ -14110,10 +14139,11 @@
         <v>38.023524999999999</v>
       </c>
       <c r="C25">
-        <v>84.509702000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.509702000000004</v>
+      </c>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -14121,10 +14151,11 @@
         <v>38.02525</v>
       </c>
       <c r="C26">
-        <v>84.510149999999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.510149999999996</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>66</v>
       </c>
@@ -14132,10 +14163,11 @@
         <v>38.025202</v>
       </c>
       <c r="C27">
-        <v>84.505421999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.505421999999996</v>
+      </c>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>67</v>
       </c>
@@ -14143,10 +14175,11 @@
         <v>38.021540000000002</v>
       </c>
       <c r="C28">
-        <v>84.507071999999994</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.507071999999994</v>
+      </c>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>68</v>
       </c>
@@ -14154,10 +14187,11 @@
         <v>38.031376999999999</v>
       </c>
       <c r="C29">
-        <v>84.510611999999995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.510611999999995</v>
+      </c>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>69</v>
       </c>
@@ -14165,10 +14199,11 @@
         <v>38.033625000000001</v>
       </c>
       <c r="C30">
-        <v>84.507394000000005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.507394000000005</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>70</v>
       </c>
@@ -14176,10 +14211,11 @@
         <v>38.042408999999999</v>
       </c>
       <c r="C31">
-        <v>84.501808999999994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.501808999999994</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>71</v>
       </c>
@@ -14187,10 +14223,11 @@
         <v>38.032350000000001</v>
       </c>
       <c r="C32">
-        <v>84.50891</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.50891</v>
+      </c>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>139</v>
       </c>
@@ -14198,10 +14235,11 @@
         <v>38.037529999999997</v>
       </c>
       <c r="C33">
-        <v>84.501649999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.501649999999998</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>73</v>
       </c>
@@ -14209,10 +14247,11 @@
         <v>38.017949999999999</v>
       </c>
       <c r="C34">
-        <v>84.505949999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.505949999999999</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>74</v>
       </c>
@@ -14220,10 +14259,11 @@
         <v>38.023788000000003</v>
       </c>
       <c r="C35">
-        <v>84.503692000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.503692000000001</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>75</v>
       </c>
@@ -14231,10 +14271,11 @@
         <v>38.025010000000002</v>
       </c>
       <c r="C36">
-        <v>84.505750000000006</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.505750000000006</v>
+      </c>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>76</v>
       </c>
@@ -14242,10 +14283,11 @@
         <v>38.028570000000002</v>
       </c>
       <c r="C37">
-        <v>84.509900000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.509900000000002</v>
+      </c>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>77</v>
       </c>
@@ -14253,10 +14295,11 @@
         <v>38.018380000000001</v>
       </c>
       <c r="C38">
-        <v>84.499570000000006</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.499570000000006</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>78</v>
       </c>
@@ -14264,10 +14307,11 @@
         <v>38.027315999999999</v>
       </c>
       <c r="C39">
-        <v>84.501604</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.501604</v>
+      </c>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>79</v>
       </c>
@@ -14275,10 +14319,11 @@
         <v>38.028190000000002</v>
       </c>
       <c r="C40">
-        <v>84.502589999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.502589999999998</v>
+      </c>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>80</v>
       </c>
@@ -14286,10 +14331,11 @@
         <v>38.02854</v>
       </c>
       <c r="C41">
-        <v>84.499080000000006</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.499080000000006</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>81</v>
       </c>
@@ -14297,10 +14343,11 @@
         <v>38.034097000000003</v>
       </c>
       <c r="C42">
-        <v>84.500164999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.500164999999996</v>
+      </c>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>82</v>
       </c>
@@ -14308,10 +14355,11 @@
         <v>38.036380000000001</v>
       </c>
       <c r="C43">
-        <v>84.500309999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.500309999999999</v>
+      </c>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>83</v>
       </c>
@@ -14319,10 +14367,11 @@
         <v>38.034419999999997</v>
       </c>
       <c r="C44">
-        <v>84.499880000000005</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.499880000000005</v>
+      </c>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>84</v>
       </c>
@@ -14330,10 +14379,11 @@
         <v>38.035690000000002</v>
       </c>
       <c r="C45">
-        <v>84.500150000000005</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.500150000000005</v>
+      </c>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>85</v>
       </c>
@@ -14341,10 +14391,11 @@
         <v>38.035170000000001</v>
       </c>
       <c r="C46">
-        <v>84.500470000000007</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.500470000000007</v>
+      </c>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>86</v>
       </c>
@@ -14352,10 +14403,11 @@
         <v>38.034869999999998</v>
       </c>
       <c r="C47">
-        <v>84.499290000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.499290000000002</v>
+      </c>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>87</v>
       </c>
@@ -14363,10 +14415,11 @@
         <v>38.038690000000003</v>
       </c>
       <c r="C48">
-        <v>84.499129999999994</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.499129999999994</v>
+      </c>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>88</v>
       </c>
@@ -14374,10 +14427,11 @@
         <v>38.039349999999999</v>
       </c>
       <c r="C49">
-        <v>84.499340000000004</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.499340000000004</v>
+      </c>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>89</v>
       </c>
@@ -14385,10 +14439,11 @@
         <v>38.018250000000002</v>
       </c>
       <c r="C50">
-        <v>84.510050000000007</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.510050000000007</v>
+      </c>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>90</v>
       </c>
@@ -14396,10 +14451,11 @@
         <v>38.037410000000001</v>
       </c>
       <c r="C51">
-        <v>84.509730000000005</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.509730000000005</v>
+      </c>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>91</v>
       </c>
@@ -14407,10 +14463,11 @@
         <v>38.043089999999999</v>
       </c>
       <c r="C52">
-        <v>84.507940000000005</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.507940000000005</v>
+      </c>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>92</v>
       </c>
@@ -14418,10 +14475,11 @@
         <v>38.043329999999997</v>
       </c>
       <c r="C53">
-        <v>84.506280000000004</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-84.506280000000004</v>
+      </c>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>93</v>
       </c>
@@ -14429,10 +14487,13 @@
         <v>38.02073</v>
       </c>
       <c r="C54">
-        <v>84.509820000000005</v>
-      </c>
+        <v>-84.509820000000005</v>
+      </c>
+      <c r="D54" s="8"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>